<commit_message>
[Fix] : generate_packets.py 출력 내용 수정
- CSector 단위로 _FOR_AROUND 형식을 만들던 함수를 CRoom 단위로 수정
</commit_message>
<xml_diff>
--- a/AllInOneGenerator/proto_definitions.xlsx
+++ b/AllInOneGenerator/proto_definitions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\FPS26Server\ProtoFileGenerator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\FPS26Server\AllInOneGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3110E39-62F4-4582-A0D4-506C359D8DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A740F817-8B15-40CC-8773-FD586F1825B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="3045" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7395" yWindow="3360" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="80">
   <si>
     <t>MessageName</t>
   </si>
@@ -254,6 +254,14 @@
   </si>
   <si>
     <t>다른 캐릭터 ID</t>
+  </si>
+  <si>
+    <t>TeamID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>접속한 팀 ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -625,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -834,18 +842,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -853,13 +861,13 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -867,7 +875,7 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
@@ -881,7 +889,7 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
@@ -895,13 +903,13 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -909,7 +917,7 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
@@ -923,7 +931,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
@@ -937,13 +945,13 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -951,7 +959,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
@@ -965,13 +973,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -979,55 +987,55 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" t="s">
         <v>32</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>8</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>34</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>14</v>
       </c>
-      <c r="C32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>36</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>37</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1035,10 +1043,13 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C37" t="s">
         <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1046,7 +1057,7 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38" t="s">
         <v>10</v>
@@ -1057,7 +1068,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
         <v>10</v>
@@ -1068,13 +1079,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
-      </c>
-      <c r="D40" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1082,13 +1090,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C41" t="s">
         <v>46</v>
       </c>
       <c r="D41" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1096,24 +1104,27 @@
         <v>39</v>
       </c>
       <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" t="s">
         <v>50</v>
       </c>
-      <c r="C42" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1121,13 +1132,10 @@
         <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C45" t="s">
         <v>10</v>
-      </c>
-      <c r="D45" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1135,10 +1143,13 @@
         <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C46" t="s">
         <v>10</v>
+      </c>
+      <c r="D46" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1146,7 +1157,7 @@
         <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" t="s">
         <v>10</v>
@@ -1157,7 +1168,7 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
         <v>10</v>
@@ -1168,13 +1179,10 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C49" t="s">
-        <v>46</v>
-      </c>
-      <c r="D49" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1182,13 +1190,13 @@
         <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
         <v>46</v>
       </c>
       <c r="D50" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1196,27 +1204,27 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
         <v>50</v>
       </c>
-      <c r="C51" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>53</v>
-      </c>
-      <c r="B53" t="s">
-        <v>18</v>
-      </c>
-      <c r="C53" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1224,10 +1232,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C54" t="s">
         <v>10</v>
+      </c>
+      <c r="D54" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1235,24 +1246,21 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
         <v>21</v>
       </c>
-      <c r="C55" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
-        <v>18</v>
-      </c>
-      <c r="C57" t="s">
-        <v>10</v>
-      </c>
-      <c r="D57" t="s">
-        <v>54</v>
+      <c r="C56" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1260,10 +1268,13 @@
         <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C58" t="s">
         <v>10</v>
+      </c>
+      <c r="D58" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1271,49 +1282,46 @@
         <v>55</v>
       </c>
       <c r="B59" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" t="s">
         <v>21</v>
       </c>
-      <c r="C59" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="C60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>56</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>57</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>58</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>60</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>14</v>
       </c>
-      <c r="C63" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>61</v>
-      </c>
-      <c r="B65" t="s">
-        <v>14</v>
-      </c>
-      <c r="C65" t="s">
-        <v>10</v>
-      </c>
-      <c r="D65" t="s">
-        <v>62</v>
+      <c r="C64" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1321,27 +1329,27 @@
         <v>61</v>
       </c>
       <c r="B66" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>61</v>
+      </c>
+      <c r="B67" t="s">
         <v>63</v>
       </c>
-      <c r="C66" t="s">
-        <v>10</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="C67" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>65</v>
-      </c>
-      <c r="B68" t="s">
-        <v>14</v>
-      </c>
-      <c r="C68" t="s">
-        <v>10</v>
-      </c>
-      <c r="D68" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1349,27 +1357,27 @@
         <v>65</v>
       </c>
       <c r="B69" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" t="s">
         <v>63</v>
       </c>
-      <c r="C69" t="s">
-        <v>10</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="D70" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>66</v>
-      </c>
-      <c r="B71" t="s">
-        <v>18</v>
-      </c>
-      <c r="C71" t="s">
-        <v>10</v>
-      </c>
-      <c r="D71" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1377,10 +1385,13 @@
         <v>66</v>
       </c>
       <c r="B72" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C72" t="s">
         <v>10</v>
+      </c>
+      <c r="D72" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1388,7 +1399,7 @@
         <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C73" t="s">
         <v>10</v>
@@ -1399,13 +1410,10 @@
         <v>66</v>
       </c>
       <c r="B74" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C74" t="s">
-        <v>46</v>
-      </c>
-      <c r="D74" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1413,10 +1421,13 @@
         <v>66</v>
       </c>
       <c r="B75" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C75" t="s">
         <v>46</v>
+      </c>
+      <c r="D75" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -1424,24 +1435,21 @@
         <v>66</v>
       </c>
       <c r="B76" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C76" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>69</v>
-      </c>
-      <c r="B78" t="s">
-        <v>18</v>
-      </c>
-      <c r="C78" t="s">
-        <v>10</v>
-      </c>
-      <c r="D78" t="s">
-        <v>67</v>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>66</v>
+      </c>
+      <c r="B77" t="s">
+        <v>25</v>
+      </c>
+      <c r="C77" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -1449,10 +1457,13 @@
         <v>69</v>
       </c>
       <c r="B79" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C79" t="s">
         <v>10</v>
+      </c>
+      <c r="D79" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -1460,7 +1471,7 @@
         <v>69</v>
       </c>
       <c r="B80" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C80" t="s">
         <v>10</v>
@@ -1471,13 +1482,10 @@
         <v>69</v>
       </c>
       <c r="B81" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C81" t="s">
-        <v>46</v>
-      </c>
-      <c r="D81" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -1485,10 +1493,13 @@
         <v>69</v>
       </c>
       <c r="B82" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C82" t="s">
         <v>46</v>
+      </c>
+      <c r="D82" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -1496,24 +1507,21 @@
         <v>69</v>
       </c>
       <c r="B83" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C83" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>70</v>
-      </c>
-      <c r="B85" t="s">
-        <v>18</v>
-      </c>
-      <c r="C85" t="s">
-        <v>10</v>
-      </c>
-      <c r="D85" t="s">
-        <v>71</v>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>69</v>
+      </c>
+      <c r="B84" t="s">
+        <v>25</v>
+      </c>
+      <c r="C84" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -1521,10 +1529,13 @@
         <v>70</v>
       </c>
       <c r="B86" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C86" t="s">
         <v>10</v>
+      </c>
+      <c r="D86" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -1532,24 +1543,21 @@
         <v>70</v>
       </c>
       <c r="B87" t="s">
+        <v>20</v>
+      </c>
+      <c r="C87" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>70</v>
+      </c>
+      <c r="B88" t="s">
         <v>21</v>
       </c>
-      <c r="C87" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>72</v>
-      </c>
-      <c r="B89" t="s">
-        <v>18</v>
-      </c>
-      <c r="C89" t="s">
-        <v>10</v>
-      </c>
-      <c r="D89" t="s">
-        <v>71</v>
+      <c r="C88" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -1557,10 +1565,13 @@
         <v>72</v>
       </c>
       <c r="B90" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C90" t="s">
         <v>10</v>
+      </c>
+      <c r="D90" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -1568,38 +1579,35 @@
         <v>72</v>
       </c>
       <c r="B91" t="s">
+        <v>20</v>
+      </c>
+      <c r="C91" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>72</v>
+      </c>
+      <c r="B92" t="s">
         <v>21</v>
       </c>
-      <c r="C91" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+      <c r="C92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>73</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>74</v>
       </c>
-      <c r="C93" t="s">
-        <v>10</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="C94" t="s">
+        <v>10</v>
+      </c>
+      <c r="D94" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>76</v>
-      </c>
-      <c r="B95" t="s">
-        <v>14</v>
-      </c>
-      <c r="C95" t="s">
-        <v>10</v>
-      </c>
-      <c r="D95" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -1607,12 +1615,26 @@
         <v>76</v>
       </c>
       <c r="B96" t="s">
+        <v>14</v>
+      </c>
+      <c r="C96" t="s">
+        <v>10</v>
+      </c>
+      <c r="D96" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>76</v>
+      </c>
+      <c r="B97" t="s">
         <v>74</v>
       </c>
-      <c r="C96" t="s">
-        <v>10</v>
-      </c>
-      <c r="D96" t="s">
+      <c r="C97" t="s">
+        <v>10</v>
+      </c>
+      <c r="D97" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Fix] : ProtoToCPPFileGenerator 수정
- generate_packet_proc.py에 CRoomManager 부분 추가
- generate_packets.py에서 pRoom의 GetActivePlayers 에게 전송하도록 FOR_AROUND 수정
</commit_message>
<xml_diff>
--- a/AllInOneGenerator/proto_definitions.xlsx
+++ b/AllInOneGenerator/proto_definitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\FPS26Server\AllInOneGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A740F817-8B15-40CC-8773-FD586F1825B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BB92A2-CD75-4C31-A464-E46CAD90E126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7395" yWindow="3360" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="111">
   <si>
     <t>MessageName</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>CS_ON_ACCEPT</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -238,9 +235,6 @@
     <t>터질 위치</t>
   </si>
   <si>
-    <t>SC_GRENADEEXPLOSITIONPOS</t>
-  </si>
-  <si>
     <t>CS_CHANGE_WEAPON</t>
   </si>
   <si>
@@ -256,11 +250,142 @@
     <t>다른 캐릭터 ID</t>
   </si>
   <si>
-    <t>TeamID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>접속한 팀 ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_SEND_NICKNAME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_ON_ACCEPT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_ATTACK을 전송한 플레이어 Id를 방에 있는 모든 플레이어들에게 전송</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_ITEM_PICKED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_ITEM_SPAWNED</t>
+  </si>
+  <si>
+    <t>itemId</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>생성될 아이템의 고유 ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>itemType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>생성될 아이템의 타입</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>itemPosIndex</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템이 생성될 장소에 대한 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템의 고유 ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>획득한 플레이어의 고유 ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_ITEM_PICK_SUCCESS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_ITEM_PICK_FAIL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>획득 시도한 아이템의 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>획득 실패한 플레이어의 고유 ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>무기 교체</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>들고 있는 무기 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>posIndex</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>생성될 위치 인덱스 정보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>normalX</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>normalY</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>normalZ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_REQUEST_RESTART</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어의 고유 ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_ATTACK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이펙트가 터질 위치</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이펙트의 노멀 벡터</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>weapon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_GRENADE_EXPLOSITION_POS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_CREATE_OTHER_CHARACTER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>teamID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>마우스 Y축 회전값</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -633,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -663,979 +788,1271 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
         <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
         <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>79</v>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
         <v>28</v>
-      </c>
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>35</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>36</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>37</v>
-      </c>
-      <c r="D35" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
         <v>39</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
         <v>40</v>
-      </c>
-      <c r="C37" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" t="s">
         <v>45</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>46</v>
-      </c>
-      <c r="D41" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" t="s">
         <v>48</v>
-      </c>
-      <c r="C42" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
         <v>50</v>
-      </c>
-      <c r="C43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D43" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" t="s">
         <v>40</v>
-      </c>
-      <c r="C46" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" t="s">
         <v>45</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>46</v>
-      </c>
-      <c r="D50" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" t="s">
+        <v>45</v>
+      </c>
+      <c r="D51" t="s">
         <v>48</v>
-      </c>
-      <c r="C51" t="s">
-        <v>46</v>
-      </c>
-      <c r="D51" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" t="s">
         <v>50</v>
-      </c>
-      <c r="C52" t="s">
-        <v>10</v>
-      </c>
-      <c r="D52" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" t="s">
         <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>18</v>
-      </c>
-      <c r="C54" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" t="s">
         <v>56</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>57</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>58</v>
       </c>
-      <c r="D62" t="s">
-        <v>59</v>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>103</v>
+      </c>
+      <c r="B63" t="s">
+        <v>98</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="B64" t="s">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="C64" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="B66" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D66" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="B67" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="C67" t="s">
-        <v>10</v>
-      </c>
-      <c r="D67" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>65</v>
-      </c>
-      <c r="B69" t="s">
-        <v>14</v>
-      </c>
-      <c r="C69" t="s">
-        <v>10</v>
-      </c>
-      <c r="D69" t="s">
-        <v>62</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>103</v>
+      </c>
+      <c r="B68" t="s">
+        <v>20</v>
+      </c>
+      <c r="C68" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B70" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="C70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D70" t="s">
-        <v>64</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" t="s">
+        <v>98</v>
+      </c>
+      <c r="C71" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B72" t="s">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="C72" t="s">
-        <v>10</v>
-      </c>
-      <c r="D72" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B73" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B74" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C74" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="D74" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B75" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C75" t="s">
-        <v>46</v>
-      </c>
-      <c r="D75" t="s">
-        <v>68</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B76" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C76" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>66</v>
-      </c>
-      <c r="B77" t="s">
-        <v>25</v>
-      </c>
-      <c r="C77" t="s">
-        <v>46</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>60</v>
+      </c>
+      <c r="B78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C78" t="s">
+        <v>9</v>
+      </c>
+      <c r="D78" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B79" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D79" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>69</v>
-      </c>
-      <c r="B80" t="s">
-        <v>20</v>
-      </c>
-      <c r="C80" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B81" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C81" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="D81" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B82" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C82" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="D82" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>69</v>
-      </c>
-      <c r="B83" t="s">
-        <v>24</v>
-      </c>
-      <c r="C83" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B84" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C84" t="s">
-        <v>46</v>
+        <v>9</v>
+      </c>
+      <c r="D84" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>65</v>
+      </c>
+      <c r="B85" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B86" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C86" t="s">
-        <v>10</v>
-      </c>
-      <c r="D86" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B87" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C87" t="s">
-        <v>10</v>
+        <v>45</v>
+      </c>
+      <c r="D87" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B88" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C88" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>72</v>
-      </c>
-      <c r="B90" t="s">
-        <v>18</v>
-      </c>
-      <c r="C90" t="s">
-        <v>10</v>
-      </c>
-      <c r="D90" t="s">
-        <v>71</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>65</v>
+      </c>
+      <c r="B89" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B91" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C91" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="D91" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B92" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C92" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>68</v>
+      </c>
+      <c r="B93" t="s">
+        <v>20</v>
+      </c>
+      <c r="C93" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B94" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="C94" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D94" t="s">
-        <v>75</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>68</v>
+      </c>
+      <c r="B95" t="s">
+        <v>23</v>
+      </c>
+      <c r="C95" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B96" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C96" t="s">
-        <v>10</v>
-      </c>
-      <c r="D96" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>69</v>
+      </c>
+      <c r="B98" t="s">
+        <v>17</v>
+      </c>
+      <c r="C98" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>69</v>
+      </c>
+      <c r="B99" t="s">
+        <v>19</v>
+      </c>
+      <c r="C99" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>69</v>
+      </c>
+      <c r="B100" t="s">
+        <v>20</v>
+      </c>
+      <c r="C100" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>107</v>
+      </c>
+      <c r="B102" t="s">
+        <v>17</v>
+      </c>
+      <c r="C102" t="s">
+        <v>9</v>
+      </c>
+      <c r="D102" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>107</v>
+      </c>
+      <c r="B103" t="s">
+        <v>19</v>
+      </c>
+      <c r="C103" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>107</v>
+      </c>
+      <c r="B104" t="s">
+        <v>20</v>
+      </c>
+      <c r="C104" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>71</v>
+      </c>
+      <c r="B106" t="s">
+        <v>72</v>
+      </c>
+      <c r="C106" t="s">
+        <v>9</v>
+      </c>
+      <c r="D106" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>74</v>
+      </c>
+      <c r="B108" t="s">
+        <v>13</v>
+      </c>
+      <c r="C108" t="s">
+        <v>9</v>
+      </c>
+      <c r="D108" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>74</v>
+      </c>
+      <c r="B109" t="s">
+        <v>106</v>
+      </c>
+      <c r="C109" t="s">
+        <v>9</v>
+      </c>
+      <c r="D109" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>76</v>
-      </c>
-      <c r="B97" t="s">
-        <v>74</v>
-      </c>
-      <c r="C97" t="s">
-        <v>10</v>
-      </c>
-      <c r="D97" t="s">
-        <v>75</v>
+      <c r="B111" t="s">
+        <v>4</v>
+      </c>
+      <c r="C111" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>81</v>
+      </c>
+      <c r="B113" t="s">
+        <v>82</v>
+      </c>
+      <c r="C113" t="s">
+        <v>9</v>
+      </c>
+      <c r="D113" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>81</v>
+      </c>
+      <c r="B114" t="s">
+        <v>84</v>
+      </c>
+      <c r="C114" t="s">
+        <v>9</v>
+      </c>
+      <c r="D114" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>81</v>
+      </c>
+      <c r="B115" t="s">
+        <v>86</v>
+      </c>
+      <c r="C115" t="s">
+        <v>9</v>
+      </c>
+      <c r="D115" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>80</v>
+      </c>
+      <c r="B117" t="s">
+        <v>82</v>
+      </c>
+      <c r="C117" t="s">
+        <v>9</v>
+      </c>
+      <c r="D117" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>90</v>
+      </c>
+      <c r="B119" t="s">
+        <v>13</v>
+      </c>
+      <c r="C119" t="s">
+        <v>9</v>
+      </c>
+      <c r="D119" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>90</v>
+      </c>
+      <c r="B120" t="s">
+        <v>82</v>
+      </c>
+      <c r="C120" t="s">
+        <v>9</v>
+      </c>
+      <c r="D120" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>91</v>
+      </c>
+      <c r="B122" t="s">
+        <v>13</v>
+      </c>
+      <c r="C122" t="s">
+        <v>9</v>
+      </c>
+      <c r="D122" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>91</v>
+      </c>
+      <c r="B123" t="s">
+        <v>82</v>
+      </c>
+      <c r="C123" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>101</v>
+      </c>
+      <c r="B125" t="s">
+        <v>13</v>
+      </c>
+      <c r="C125" t="s">
+        <v>9</v>
+      </c>
+      <c r="D125" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>101</v>
+      </c>
+      <c r="B126" t="s">
+        <v>106</v>
+      </c>
+      <c r="C126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D126" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Feat] : AllInOneGenerator에 Protocol.proto 파일까지 자동화 하는 기능 추가
</commit_message>
<xml_diff>
--- a/AllInOneGenerator/proto_definitions.xlsx
+++ b/AllInOneGenerator/proto_definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\FPS26Server\AllInOneGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7399167F-BE2D-498C-8D03-5E867277EBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DC4027-940B-480F-98C8-E16B4F454625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="114">
   <si>
     <t>MessageName</t>
   </si>
@@ -380,6 +380,26 @@
   </si>
   <si>
     <t>SC_CHARACTER_DOWN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SC_SEND_MESSAGE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CS_SEND_MESSAGE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>message</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전송할 문자열</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -752,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -782,16 +802,24 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -799,54 +827,46 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1955,6 +1975,62 @@
       </c>
       <c r="D119" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>109</v>
+      </c>
+      <c r="B121" t="s">
+        <v>13</v>
+      </c>
+      <c r="C121" t="s">
+        <v>9</v>
+      </c>
+      <c r="D121" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>109</v>
+      </c>
+      <c r="B122" t="s">
+        <v>111</v>
+      </c>
+      <c r="C122" t="s">
+        <v>112</v>
+      </c>
+      <c r="D122" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>110</v>
+      </c>
+      <c r="B124" t="s">
+        <v>13</v>
+      </c>
+      <c r="C124" t="s">
+        <v>9</v>
+      </c>
+      <c r="D124" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>110</v>
+      </c>
+      <c r="B125" t="s">
+        <v>111</v>
+      </c>
+      <c r="C125" t="s">
+        <v>112</v>
+      </c>
+      <c r="D125" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Feat] : CS_ATTACK, SC_POS_INTERPOLATION 프로토콜 수정
</commit_message>
<xml_diff>
--- a/AllInOneGenerator/proto_definitions.xlsx
+++ b/AllInOneGenerator/proto_definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\FPS26Server\AllInOneGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4BED7E-0529-46B7-9A1E-0E1B142E1063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B509CC24-1E1B-4832-A814-65BF0BA213B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="105">
   <si>
     <t>MessageName</t>
   </si>
@@ -175,15 +175,6 @@
     <t>CS_ATTACK</t>
   </si>
   <si>
-    <t>bAttack</t>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>임의의 변수, 의미 없음.</t>
-  </si>
-  <si>
     <t>SC_ATTACK</t>
   </si>
   <si>
@@ -373,6 +364,18 @@
   </si>
   <si>
     <t>float</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어의 현재 위치</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어 Id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hittedTargetId</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -745,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -830,7 +833,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -861,13 +864,13 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -889,13 +892,13 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -917,13 +920,13 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -981,35 +984,35 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
@@ -1026,13 +1029,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1246,10 +1249,10 @@
         <v>17</v>
       </c>
       <c r="C47" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D47" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1260,7 +1263,7 @@
         <v>18</v>
       </c>
       <c r="C48" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1271,7 +1274,7 @@
         <v>19</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1279,13 +1282,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1293,10 +1296,13 @@
         <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="D52" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1304,358 +1310,369 @@
         <v>49</v>
       </c>
       <c r="B53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" t="s">
         <v>19</v>
       </c>
-      <c r="C53" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>50</v>
-      </c>
-      <c r="B55" t="s">
-        <v>51</v>
-      </c>
-      <c r="C55" t="s">
-        <v>52</v>
-      </c>
-      <c r="D55" t="s">
-        <v>53</v>
+      <c r="C54" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
       <c r="B56" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="C56" t="s">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="D56" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B57" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C57" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="D57" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B58" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C58" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B59" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="C59" t="s">
-        <v>104</v>
-      </c>
-      <c r="D59" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C60" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="D60" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B61" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" t="s">
         <v>19</v>
       </c>
-      <c r="C61" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>54</v>
-      </c>
-      <c r="B63" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" t="s">
-        <v>9</v>
-      </c>
-      <c r="D63" t="s">
-        <v>68</v>
+      <c r="C62" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B64" t="s">
-        <v>87</v>
+        <v>13</v>
       </c>
       <c r="C64" t="s">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="D64" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B65" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="C65" t="s">
-        <v>104</v>
+        <v>9</v>
+      </c>
+      <c r="D65" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C66" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="D66" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B67" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="C67" t="s">
-        <v>104</v>
-      </c>
-      <c r="D67" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B68" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="C68" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C69" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="D69" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>51</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B71" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>52</v>
+      </c>
+      <c r="B73" t="s">
         <v>13</v>
       </c>
-      <c r="C71" t="s">
-        <v>9</v>
-      </c>
-      <c r="D71" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>55</v>
-      </c>
-      <c r="B72" t="s">
-        <v>57</v>
-      </c>
-      <c r="C72" t="s">
-        <v>9</v>
-      </c>
-      <c r="D72" t="s">
-        <v>58</v>
+      <c r="C73" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B74" t="s">
+        <v>54</v>
+      </c>
+      <c r="C74" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>56</v>
+      </c>
+      <c r="B76" t="s">
         <v>13</v>
       </c>
-      <c r="C74" t="s">
-        <v>9</v>
-      </c>
-      <c r="D74" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>59</v>
-      </c>
-      <c r="B75" t="s">
-        <v>57</v>
-      </c>
-      <c r="C75" t="s">
-        <v>9</v>
-      </c>
-      <c r="D75" t="s">
-        <v>58</v>
+      <c r="C76" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B77" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C77" t="s">
         <v>9</v>
       </c>
       <c r="D77" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B79" t="s">
+        <v>58</v>
+      </c>
+      <c r="C79" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>60</v>
+      </c>
+      <c r="B81" t="s">
         <v>13</v>
       </c>
-      <c r="C79" t="s">
-        <v>9</v>
-      </c>
-      <c r="D79" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>63</v>
-      </c>
-      <c r="B80" t="s">
-        <v>95</v>
-      </c>
-      <c r="C80" t="s">
-        <v>9</v>
-      </c>
-      <c r="D80" t="s">
-        <v>62</v>
+      <c r="C81" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="C82" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D82" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B84" t="s">
-        <v>71</v>
+        <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D84" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>70</v>
-      </c>
-      <c r="B85" t="s">
-        <v>73</v>
-      </c>
-      <c r="C85" t="s">
-        <v>9</v>
-      </c>
-      <c r="D85" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
+        <v>67</v>
+      </c>
+      <c r="B86" t="s">
+        <v>68</v>
+      </c>
+      <c r="C86" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>67</v>
+      </c>
+      <c r="B87" t="s">
         <v>70</v>
       </c>
-      <c r="B86" t="s">
-        <v>75</v>
-      </c>
-      <c r="C86" t="s">
-        <v>9</v>
-      </c>
-      <c r="D86" t="s">
-        <v>76</v>
+      <c r="C87" t="s">
+        <v>9</v>
+      </c>
+      <c r="D87" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B88" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C88" t="s">
         <v>9</v>
       </c>
       <c r="D88" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B90" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="C90" t="s">
         <v>9</v>
@@ -1664,130 +1681,144 @@
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>79</v>
-      </c>
-      <c r="B91" t="s">
-        <v>71</v>
-      </c>
-      <c r="C91" t="s">
-        <v>9</v>
-      </c>
-      <c r="D91" t="s">
-        <v>77</v>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>76</v>
+      </c>
+      <c r="B92" t="s">
+        <v>13</v>
+      </c>
+      <c r="C92" t="s">
+        <v>9</v>
+      </c>
+      <c r="D92" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B93" t="s">
+        <v>68</v>
+      </c>
+      <c r="C93" t="s">
+        <v>9</v>
+      </c>
+      <c r="D93" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>77</v>
+      </c>
+      <c r="B95" t="s">
         <v>13</v>
       </c>
-      <c r="C93" t="s">
-        <v>9</v>
-      </c>
-      <c r="D93" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>80</v>
-      </c>
-      <c r="B94" t="s">
-        <v>71</v>
-      </c>
-      <c r="C94" t="s">
-        <v>9</v>
-      </c>
-      <c r="D94" t="s">
-        <v>77</v>
+      <c r="C95" t="s">
+        <v>9</v>
+      </c>
+      <c r="D95" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B96" t="s">
+        <v>68</v>
+      </c>
+      <c r="C96" t="s">
+        <v>9</v>
+      </c>
+      <c r="D96" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>87</v>
+      </c>
+      <c r="B98" t="s">
         <v>13</v>
       </c>
-      <c r="C96" t="s">
-        <v>9</v>
-      </c>
-      <c r="D96" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>90</v>
-      </c>
-      <c r="B97" t="s">
-        <v>95</v>
-      </c>
-      <c r="C97" t="s">
-        <v>9</v>
-      </c>
-      <c r="D97" t="s">
-        <v>84</v>
+      <c r="C98" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B99" t="s">
+        <v>92</v>
+      </c>
+      <c r="C99" t="s">
+        <v>9</v>
+      </c>
+      <c r="D99" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>96</v>
+      </c>
+      <c r="B101" t="s">
         <v>13</v>
       </c>
-      <c r="C99" t="s">
-        <v>9</v>
-      </c>
-      <c r="D99" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>99</v>
-      </c>
-      <c r="B100" t="s">
-        <v>101</v>
-      </c>
-      <c r="C100" t="s">
-        <v>102</v>
-      </c>
-      <c r="D100" t="s">
-        <v>103</v>
+      <c r="C101" t="s">
+        <v>9</v>
+      </c>
+      <c r="D101" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>96</v>
+      </c>
+      <c r="B102" t="s">
+        <v>98</v>
+      </c>
+      <c r="C102" t="s">
+        <v>99</v>
+      </c>
+      <c r="D102" t="s">
         <v>100</v>
       </c>
-      <c r="B102" t="s">
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>97</v>
+      </c>
+      <c r="B104" t="s">
         <v>13</v>
       </c>
-      <c r="C102" t="s">
-        <v>9</v>
-      </c>
-      <c r="D102" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+      <c r="C104" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>97</v>
+      </c>
+      <c r="B105" t="s">
+        <v>98</v>
+      </c>
+      <c r="C105" t="s">
+        <v>99</v>
+      </c>
+      <c r="D105" t="s">
         <v>100</v>
-      </c>
-      <c r="B103" t="s">
-        <v>101</v>
-      </c>
-      <c r="C103" t="s">
-        <v>102</v>
-      </c>
-      <c r="D103" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Fix] : KeyInput 프로토콜 수정
- normal값 추가
- wasd key 입력을 bool 변수로 전달
- fixed32 사용 x
</commit_message>
<xml_diff>
--- a/AllInOneGenerator/proto_definitions.xlsx
+++ b/AllInOneGenerator/proto_definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Sparta\FPS26Server\AllInOneGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B509CC24-1E1B-4832-A814-65BF0BA213B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1103D921-6FEC-40B3-B1A1-A29D4C150872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="106">
   <si>
     <t>MessageName</t>
   </si>
@@ -142,9 +142,6 @@
     <t>rotateAxisX</t>
   </si>
   <si>
-    <t>fixed32</t>
-  </si>
-  <si>
     <t>마우스 X축 회전값</t>
   </si>
   <si>
@@ -376,6 +373,14 @@
   </si>
   <si>
     <t>hittedTargetId</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어의 노멀 벡터</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -748,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -833,7 +838,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -864,13 +869,13 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
         <v>82</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -892,13 +897,13 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -920,13 +925,13 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
         <v>82</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -984,35 +989,35 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" t="s">
         <v>93</v>
       </c>
-      <c r="B23" t="s">
-        <v>94</v>
-      </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" t="s">
         <v>13</v>
@@ -1029,13 +1034,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1060,7 +1065,7 @@
         <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="D30" t="s">
         <v>35</v>
@@ -1074,7 +1079,7 @@
         <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1085,7 +1090,7 @@
         <v>37</v>
       </c>
       <c r="C32" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1096,7 +1101,7 @@
         <v>38</v>
       </c>
       <c r="C33" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1107,10 +1112,10 @@
         <v>39</v>
       </c>
       <c r="C34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" t="s">
         <v>40</v>
-      </c>
-      <c r="D34" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1118,13 +1123,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" t="s">
+        <v>100</v>
+      </c>
+      <c r="D35" t="s">
         <v>42</v>
-      </c>
-      <c r="C35" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1132,57 +1137,57 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
         <v>44</v>
       </c>
-      <c r="C36" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" t="s">
-        <v>45</v>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="C39" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="C41" t="s">
         <v>9</v>
@@ -1190,556 +1195,572 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>9</v>
+        <v>105</v>
+      </c>
+      <c r="D42" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
-      </c>
-      <c r="D44" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D47" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>9</v>
+      </c>
+      <c r="D48" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="D49" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="C51" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" t="s">
-        <v>17</v>
-      </c>
-      <c r="C52" t="s">
-        <v>101</v>
-      </c>
-      <c r="D52" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B53" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C53" t="s">
+        <v>100</v>
+      </c>
+      <c r="D53" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" t="s">
         <v>19</v>
       </c>
-      <c r="C54" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>50</v>
-      </c>
-      <c r="B56" t="s">
-        <v>104</v>
-      </c>
-      <c r="C56" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" t="s">
-        <v>53</v>
+      <c r="C55" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>84</v>
+        <v>13</v>
       </c>
       <c r="C57" t="s">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="D57" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="B58" t="s">
-        <v>85</v>
+        <v>17</v>
       </c>
       <c r="C58" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="D58" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>18</v>
       </c>
       <c r="C59" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>101</v>
-      </c>
-      <c r="D60" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>89</v>
-      </c>
-      <c r="B61" t="s">
-        <v>18</v>
-      </c>
-      <c r="C61" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="B62" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="C62" t="s">
-        <v>101</v>
+        <v>9</v>
+      </c>
+      <c r="D62" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" t="s">
+        <v>100</v>
+      </c>
+      <c r="D63" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="C64" t="s">
-        <v>9</v>
-      </c>
-      <c r="D64" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="B65" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="C65" t="s">
-        <v>9</v>
-      </c>
-      <c r="D65" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="B66" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="C66" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D66" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="B67" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="C67" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="B68" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="C68" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>51</v>
-      </c>
-      <c r="B69" t="s">
-        <v>17</v>
-      </c>
-      <c r="C69" t="s">
-        <v>101</v>
-      </c>
-      <c r="D69" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B70" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C70" t="s">
-        <v>101</v>
+        <v>9</v>
+      </c>
+      <c r="D70" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B71" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="C71" t="s">
-        <v>101</v>
+        <v>9</v>
+      </c>
+      <c r="D71" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>50</v>
+      </c>
+      <c r="B72" t="s">
+        <v>83</v>
+      </c>
+      <c r="C72" t="s">
+        <v>100</v>
+      </c>
+      <c r="D72" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="C73" t="s">
-        <v>9</v>
-      </c>
-      <c r="D73" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B74" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="C74" t="s">
-        <v>9</v>
-      </c>
-      <c r="D74" t="s">
-        <v>55</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>50</v>
+      </c>
+      <c r="B75" t="s">
+        <v>17</v>
+      </c>
+      <c r="C75" t="s">
+        <v>100</v>
+      </c>
+      <c r="D75" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B76" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C76" t="s">
-        <v>9</v>
-      </c>
-      <c r="D76" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B77" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
-      </c>
-      <c r="D77" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B79" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="C79" t="s">
         <v>9</v>
       </c>
       <c r="D79" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>60</v>
-      </c>
-      <c r="B81" t="s">
-        <v>13</v>
-      </c>
-      <c r="C81" t="s">
-        <v>9</v>
-      </c>
-      <c r="D81" t="s">
-        <v>61</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>51</v>
+      </c>
+      <c r="B80" t="s">
+        <v>53</v>
+      </c>
+      <c r="C80" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B82" t="s">
-        <v>92</v>
+        <v>13</v>
       </c>
       <c r="C82" t="s">
         <v>9</v>
       </c>
       <c r="D82" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>63</v>
-      </c>
-      <c r="B84" t="s">
-        <v>4</v>
-      </c>
-      <c r="C84" t="s">
-        <v>5</v>
-      </c>
-      <c r="D84" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>67</v>
-      </c>
-      <c r="B86" t="s">
-        <v>68</v>
-      </c>
-      <c r="C86" t="s">
-        <v>9</v>
-      </c>
-      <c r="D86" t="s">
-        <v>69</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>55</v>
+      </c>
+      <c r="B83" t="s">
+        <v>53</v>
+      </c>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>56</v>
+      </c>
+      <c r="B85" t="s">
+        <v>57</v>
+      </c>
+      <c r="C85" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B87" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="C87" t="s">
         <v>9</v>
       </c>
       <c r="D87" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B88" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="C88" t="s">
         <v>9</v>
       </c>
       <c r="D88" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B90" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D90" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B92" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="C92" t="s">
         <v>9</v>
       </c>
       <c r="D92" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B93" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C93" t="s">
         <v>9</v>
       </c>
       <c r="D93" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>77</v>
-      </c>
-      <c r="B95" t="s">
-        <v>13</v>
-      </c>
-      <c r="C95" t="s">
-        <v>9</v>
-      </c>
-      <c r="D95" t="s">
-        <v>79</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>66</v>
+      </c>
+      <c r="B94" t="s">
+        <v>71</v>
+      </c>
+      <c r="C94" t="s">
+        <v>9</v>
+      </c>
+      <c r="D94" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
+        <v>65</v>
+      </c>
+      <c r="B96" t="s">
+        <v>67</v>
+      </c>
+      <c r="C96" t="s">
+        <v>9</v>
+      </c>
+      <c r="D96" t="s">
         <v>77</v>
-      </c>
-      <c r="B96" t="s">
-        <v>68</v>
-      </c>
-      <c r="C96" t="s">
-        <v>9</v>
-      </c>
-      <c r="D96" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B98" t="s">
         <v>13</v>
@@ -1748,26 +1769,26 @@
         <v>9</v>
       </c>
       <c r="D98" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B99" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="C99" t="s">
         <v>9</v>
       </c>
       <c r="D99" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B101" t="s">
         <v>13</v>
@@ -1776,26 +1797,26 @@
         <v>9</v>
       </c>
       <c r="D101" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B102" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="C102" t="s">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="D102" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B104" t="s">
         <v>13</v>
@@ -1804,21 +1825,77 @@
         <v>9</v>
       </c>
       <c r="D104" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
+        <v>86</v>
+      </c>
+      <c r="B105" t="s">
+        <v>91</v>
+      </c>
+      <c r="C105" t="s">
+        <v>9</v>
+      </c>
+      <c r="D105" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>95</v>
+      </c>
+      <c r="B107" t="s">
+        <v>13</v>
+      </c>
+      <c r="C107" t="s">
+        <v>9</v>
+      </c>
+      <c r="D107" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>95</v>
+      </c>
+      <c r="B108" t="s">
         <v>97</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C108" t="s">
         <v>98</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D108" t="s">
         <v>99</v>
       </c>
-      <c r="D105" t="s">
-        <v>100</v>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>96</v>
+      </c>
+      <c r="B110" t="s">
+        <v>13</v>
+      </c>
+      <c r="C110" t="s">
+        <v>9</v>
+      </c>
+      <c r="D110" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>96</v>
+      </c>
+      <c r="B111" t="s">
+        <v>97</v>
+      </c>
+      <c r="C111" t="s">
+        <v>98</v>
+      </c>
+      <c r="D111" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>